<commit_message>
Load data from SQL Database on page load
</commit_message>
<xml_diff>
--- a/SampleDataFile.xlsx
+++ b/SampleDataFile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\insin\Downloads\H2Input\H2Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\insin\source\repos\kuldeepsingh-in\UploadExceltoSQL.NET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCEA4E5-8C76-489D-9F8C-649C2E99FCB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C68FC6-B649-49F0-9410-C5DD403851DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
-    <t>Category1</t>
-  </si>
-  <si>
     <t>Case 1</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>Category02</t>
+  </si>
+  <si>
+    <t>Category01</t>
   </si>
 </sst>
 </file>
@@ -307,9 +307,6 @@
   </cellStyleXfs>
   <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -404,6 +401,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -689,7 +689,7 @@
   <dimension ref="A2:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -707,338 +707,338 @@
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+    </row>
+    <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="5">
+        <v>450</v>
+      </c>
+      <c r="C4" s="6">
+        <v>600000000</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="6">
+        <v>600000000</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="6">
+        <v>600000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="6">
-        <v>450</v>
-      </c>
-      <c r="C4" s="7">
-        <v>600000000</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="7">
-        <v>600000000</v>
-      </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="7">
-        <v>600000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="B5" s="5">
+        <v>20</v>
+      </c>
+      <c r="C5" s="6">
+        <v>50000000</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="6">
+        <v>50000000</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="6">
+        <v>50000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B6" s="12">
+        <v>275000</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="12">
+        <v>275000</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="12">
+        <v>1100</v>
+      </c>
+      <c r="C8" s="15">
+        <v>244410794</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="15">
+        <v>244410794</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="15">
+        <v>244410794</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="5">
+        <v>142</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="5">
+        <v>147</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1200</v>
+      </c>
+      <c r="C11" s="15">
+        <v>1000000000</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="15">
+        <v>1000000000</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="15">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="18">
+        <v>105000</v>
+      </c>
+      <c r="C12" s="19">
+        <v>50000000</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="19">
+        <v>50000000</v>
+      </c>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="19">
+        <v>50000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="7">
-        <v>50000000</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="7">
-        <v>50000000</v>
-      </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="7">
-        <v>50000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="13">
-        <v>275000</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="13">
-        <v>275000</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="13">
-        <v>1100</v>
-      </c>
-      <c r="C8" s="16">
-        <v>244410794</v>
-      </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="16">
-        <v>244410794</v>
-      </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="16">
-        <v>244410794</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="6">
-        <v>142</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="6">
-        <v>147</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1200</v>
-      </c>
-      <c r="C11" s="16">
-        <v>1000000000</v>
-      </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="16">
-        <v>1000000000</v>
-      </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="16">
-        <v>1000000000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="19">
-        <v>105000</v>
-      </c>
-      <c r="C12" s="20">
-        <v>50000000</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="20">
-        <v>50000000</v>
-      </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="20">
-        <v>50000000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="24"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="23"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E14" s="12"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="25"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="24"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="12"/>
-      <c r="H15" s="12"/>
+        <v>21</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="H15" s="11"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="26">
+      <c r="A16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="25">
         <v>3000</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="26">
         <f>B16*1000*40</f>
         <v>120000000</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="28"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="27"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="15">
+      <c r="A17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="14">
         <v>3100</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <f>B17*1000*40</f>
         <v>124000000</v>
       </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="29"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="28"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="31">
+      <c r="A18" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="30">
         <v>315000000</v>
       </c>
-      <c r="D18" s="32"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="30"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="I19" s="33"/>
+      <c r="A19" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="I19" s="32"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="23"/>
-      <c r="F21" s="24"/>
-      <c r="I21" s="24"/>
+      <c r="A21" s="22"/>
+      <c r="F21" s="23"/>
+      <c r="I21" s="23"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C22" s="34"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>